<commit_message>
1st agent working with bugs
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Techgropse/FalconFullstack/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A13CE50-B348-D741-9B7F-CF4584428BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B604886-32DC-0741-8419-7B12BDCA7FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14860" yWindow="840" windowWidth="14000" windowHeight="17180" xr2:uid="{1FF29DA3-7862-3F48-944E-A3313B4FE482}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" xr2:uid="{1FF29DA3-7862-3F48-944E-A3313B4FE482}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
   <si>
     <t>order</t>
   </si>
@@ -64,9 +64,6 @@
     <t>price per unit</t>
   </si>
   <si>
-    <t>expected amt</t>
-  </si>
-  <si>
     <t>address</t>
   </si>
   <si>
@@ -82,12 +79,6 @@
     <t>packaging pref</t>
   </si>
   <si>
-    <t>additional info</t>
-  </si>
-  <si>
-    <t>document upload</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -100,9 +91,6 @@
     <t>from db</t>
   </si>
   <si>
-    <t>Fetch</t>
-  </si>
-  <si>
     <t>user input</t>
   </si>
   <si>
@@ -112,14 +100,80 @@
     <t>set by seller</t>
   </si>
   <si>
-    <t>user account</t>
+    <t>delivery date</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>not unique</t>
+  </si>
+  <si>
+    <t>same list for all</t>
+  </si>
+  <si>
+    <t>(KG/TON)</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>expected price</t>
+  </si>
+  <si>
+    <t>fetch from user account</t>
+  </si>
+  <si>
+    <t>choose from list</t>
+  </si>
+  <si>
+    <t>must be after today</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>printed by AI from JSON</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>Agent num</t>
+  </si>
+  <si>
+    <t>LC / TT / cash</t>
+  </si>
+  <si>
+    <t>Ex Factory/deliver to Buyer factory</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>bulk_tanker/pp_bag/jerry can/drum</t>
+  </si>
+  <si>
+    <t>per unit * quantity</t>
+  </si>
+  <si>
+    <t>multiplication</t>
+  </si>
+  <si>
+    <t>2 or 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -138,6 +192,17 @@
       <color rgb="FF00B050"/>
       <name val="Webdings"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri Light (Headings)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -160,10 +225,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,292 +546,411 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE0C4FD-1744-F24A-B455-8C809C88055F}">
-  <dimension ref="A9:F24"/>
+  <dimension ref="A9:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="182" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
       <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>2</v>
       </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
+      <c r="C11" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>17</v>
+      <c r="C14" t="s">
+        <v>25</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>17</v>
+      <c r="C15" t="s">
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>17</v>
+      <c r="C16" t="s">
+        <v>26</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>17</v>
+      <c r="C22" t="s">
+        <v>40</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2nd agent working with bugs
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/Techgropse/FalconFullstack/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B604886-32DC-0741-8419-7B12BDCA7FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37EFCE64-8522-8A4A-AA72-68F83082F4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="29400" windowHeight="18460" xr2:uid="{1FF29DA3-7862-3F48-944E-A3313B4FE482}"/>
+    <workbookView xWindow="15200" yWindow="660" windowWidth="14200" windowHeight="18460" xr2:uid="{1FF29DA3-7862-3F48-944E-A3313B4FE482}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="47">
   <si>
     <t>order</t>
   </si>
@@ -166,7 +166,16 @@
     <t>multiplication</t>
   </si>
   <si>
-    <t>2 or 3</t>
+    <t>request</t>
+  </si>
+  <si>
+    <t>order/ppr/sample/quote</t>
+  </si>
+  <si>
+    <t>user select</t>
+  </si>
+  <si>
+    <t>select</t>
   </si>
 </sst>
 </file>
@@ -546,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE0C4FD-1744-F24A-B455-8C809C88055F}">
-  <dimension ref="A9:H24"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="182" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,41 +568,249 @@
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+    </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9">
         <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>14</v>
@@ -607,19 +824,19 @@
       <c r="G10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>39</v>
+      <c r="H10">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>14</v>
@@ -631,21 +848,21 @@
         <v>14</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
@@ -657,47 +874,47 @@
         <v>14</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="H13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
@@ -709,7 +926,7 @@
         <v>14</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="H14">
         <v>2</v>
@@ -720,21 +937,21 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H15">
@@ -743,216 +960,34 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H4:H16">
+    <sortCondition ref="H4:H16"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>